<commit_message>
Bug Fix and README
</commit_message>
<xml_diff>
--- a/Data/Elenco offerta Complete.xlsx
+++ b/Data/Elenco offerta Complete.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrea/Desktop/UNIVERSITÀ/CORSI/Metodi e Modelli per il Supporto alle Decisioni/Progetto/MMSD-Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDD198C-C2F2-DA46-BC97-DF530D51824F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3DAC51-DA3E-BD49-9D69-07BDECE3CBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio2" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3299" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3306" uniqueCount="647">
   <si>
     <t>Area</t>
   </si>
@@ -1966,13 +1966,32 @@
   </si>
   <si>
     <t>TECNICHE DI NEUROFISIOPATOLOGIA</t>
+  </si>
+  <si>
+    <t>LEGENDA:</t>
+  </si>
+  <si>
+    <t>Number of Students Gradueted in 2021/22. Obtained by dividing the total number of graduates in the department by the number of degrees provided by the department.</t>
+  </si>
+  <si>
+    <t>Distribution of Graduates</t>
+  </si>
+  <si>
+    <t>Percentage of students graduating in this degree, calculated based on the total number of students graduated in 2021/22 in that type of degree
+For example, 2.83 percent of total bachelor's degrees (2021/22) were earned by computer science students.</t>
+  </si>
+  <si>
+    <t>Partecipants</t>
+  </si>
+  <si>
+    <t>Number of Student enrolled to a specific degree, calculated based on the Distribution of Graduates.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2017,8 +2036,18 @@
       <color rgb="FF000000"/>
       <name val="DM Sans 14pt"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="DM Sans 14pt"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="DM Sans 14pt"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2049,8 +2078,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -2130,11 +2171,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2226,6 +2278,39 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3043,8 +3128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView zoomScale="72" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:M164"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4:W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.796875" defaultRowHeight="25"/>
@@ -3064,7 +3149,11 @@
     <col min="13" max="13" width="45.796875" style="8" customWidth="1"/>
     <col min="14" max="16" width="24.796875" style="8"/>
     <col min="17" max="17" width="55.19921875" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="24.796875" style="8"/>
+    <col min="18" max="20" width="24.796875" style="8"/>
+    <col min="21" max="21" width="56.3984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="42.796875" style="8" customWidth="1"/>
+    <col min="23" max="23" width="49" style="8" customWidth="1"/>
+    <col min="24" max="16384" width="24.796875" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="52">
@@ -3233,7 +3322,7 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
     </row>
-    <row r="4" spans="1:26" ht="78">
+    <row r="4" spans="1:26" ht="65" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>43</v>
       </c>
@@ -3284,14 +3373,16 @@
       <c r="R4" s="33"/>
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
+      <c r="U4" s="34" t="s">
+        <v>641</v>
+      </c>
+      <c r="V4" s="35"/>
+      <c r="W4" s="36"/>
       <c r="X4" s="11"/>
       <c r="Y4" s="11"/>
       <c r="Z4" s="11"/>
     </row>
-    <row r="5" spans="1:26" ht="46" customHeight="1">
+    <row r="5" spans="1:26" ht="78">
       <c r="A5" s="9" t="s">
         <v>544</v>
       </c>
@@ -3345,14 +3436,18 @@
       </c>
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
+      <c r="U5" s="37" t="s">
+        <v>605</v>
+      </c>
+      <c r="V5" s="38" t="s">
+        <v>642</v>
+      </c>
+      <c r="W5" s="39"/>
       <c r="X5" s="11"/>
       <c r="Y5" s="11"/>
       <c r="Z5" s="11"/>
     </row>
-    <row r="6" spans="1:26" ht="46" customHeight="1">
+    <row r="6" spans="1:26" ht="78">
       <c r="A6" s="9" t="s">
         <v>449</v>
       </c>
@@ -3406,9 +3501,13 @@
       </c>
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
+      <c r="U6" s="37" t="s">
+        <v>643</v>
+      </c>
+      <c r="V6" s="40" t="s">
+        <v>644</v>
+      </c>
+      <c r="W6" s="41"/>
       <c r="X6" s="11"/>
       <c r="Y6" s="11"/>
       <c r="Z6" s="11"/>
@@ -3467,9 +3566,13 @@
       </c>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
+      <c r="U7" s="42" t="s">
+        <v>645</v>
+      </c>
+      <c r="V7" s="43" t="s">
+        <v>646</v>
+      </c>
+      <c r="W7" s="44"/>
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
       <c r="Z7" s="11"/>
@@ -12179,7 +12282,7 @@
         <v>12</v>
       </c>
       <c r="M162" s="10">
-        <f t="shared" ref="M162:M193" si="10">ROUND((L162*100) / IF(C162="CU", R$7, IF(C162="II°", R$6, IF(C162="I°", R$5))), 2)</f>
+        <f t="shared" ref="M162:M164" si="10">ROUND((L162*100) / IF(C162="CU", R$7, IF(C162="II°", R$6, IF(C162="I°", R$5))), 2)</f>
         <v>0.24</v>
       </c>
       <c r="N162" s="11"/>
@@ -19780,8 +19883,12 @@
       <c r="F998" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="V7:W7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -19795,7 +19902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AC35EF-B591-FC49-BB68-B19769919CC9}">
   <dimension ref="A1:M164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="E12" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>